<commit_message>
Finalized sch and exported to layout
</commit_message>
<xml_diff>
--- a/bom_panel.xlsx
+++ b/bom_panel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erudy/work/audio-power-amplifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5DCEA3-9B41-C84C-9AD9-B5838F4CAF87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A572EFAD-E322-0340-90EB-0F3CE113FCC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33780" yWindow="2120" windowWidth="26020" windowHeight="16440" xr2:uid="{8D4FBC5B-1539-A94D-B39E-707D1787DD7B}"/>
   </bookViews>
@@ -493,7 +493,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Changed power input to use quick connect plugs
</commit_message>
<xml_diff>
--- a/bom_panel.xlsx
+++ b/bom_panel.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erudy/work/audio-power-amplifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A572EFAD-E322-0340-90EB-0F3CE113FCC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B94326F-497A-B44D-8A00-EC53E175A9E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33780" yWindow="2120" windowWidth="26020" windowHeight="16440" xr2:uid="{8D4FBC5B-1539-A94D-B39E-707D1787DD7B}"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="27260" windowHeight="17200" xr2:uid="{8D4FBC5B-1539-A94D-B39E-707D1787DD7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Description</t>
   </si>
@@ -41,24 +41,12 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Power distribution wire</t>
-  </si>
-  <si>
-    <t>2 (1 Pair Twisted) Conductor Multi-Conductor Cable  12 AWG  Enter Number of Feet in Order Quantity</t>
-  </si>
-  <si>
-    <t>55A0121-12-9/96CS2275</t>
-  </si>
-  <si>
     <t>MPN</t>
   </si>
   <si>
     <t>DPN</t>
   </si>
   <si>
-    <t>55A0121-12-9/96CS2275-DS-ND</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -71,9 +59,6 @@
     <t>Item</t>
   </si>
   <si>
-    <t>Input wire</t>
-  </si>
-  <si>
     <t>2 Conductor Multi-Conductor Cable White 22 AWG Foil 25.00' (7.62m)</t>
   </si>
   <si>
@@ -86,9 +71,6 @@
     <t>7/30 strands</t>
   </si>
   <si>
-    <t>qt in feet</t>
-  </si>
-  <si>
     <t>Potentiometer</t>
   </si>
   <si>
@@ -122,26 +104,91 @@
     <t>heat shrink (Audio input)</t>
   </si>
   <si>
-    <t>heat shrink (power input)</t>
-  </si>
-  <si>
     <t>4.8 mm Quick Connect</t>
   </si>
   <si>
     <t>Power Entry Connector Receptacle, Male Blades - Module IEC 320-C14 Panel Mount, Snap-In</t>
   </si>
   <si>
-    <t>Blade Connector (power input)</t>
+    <t>Crimping tool</t>
+  </si>
+  <si>
+    <t>CT-4071-1R</t>
+  </si>
+  <si>
+    <t>CT-4071-1R-ND</t>
+  </si>
+  <si>
+    <t>Ring terminals</t>
+  </si>
+  <si>
+    <t>will use insulated quick connect</t>
+  </si>
+  <si>
+    <t>Fuse</t>
+  </si>
+  <si>
+    <t>2-520181-2</t>
+  </si>
+  <si>
+    <t>0.187" (4.75mm) Quick Connect Female 18-22 AWG Crimp Connector Fully Insulated</t>
+  </si>
+  <si>
+    <t>A27804CT-ND</t>
+  </si>
+  <si>
+    <t>A27831-ND</t>
+  </si>
+  <si>
+    <t>4-520448-2</t>
+  </si>
+  <si>
+    <t>0.250" (6.35mm) Quick Connect Female 10-12 AWG Crimp Connector Fully Insulated</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>Panel IO</t>
+  </si>
+  <si>
+    <t>Harness</t>
+  </si>
+  <si>
+    <t>Audio Input wire</t>
+  </si>
+  <si>
+    <t>Quick Connect - Female (power input)</t>
+  </si>
+  <si>
+    <t>Quick Connect - Female (power distribution)</t>
+  </si>
+  <si>
+    <t>Quick Connect - Male (power)</t>
+  </si>
+  <si>
+    <t>A100452CT-ND</t>
+  </si>
+  <si>
+    <t>1217861-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,16 +199,36 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -169,15 +236,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -490,15 +592,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E91B0B06-BA42-2340-A589-1662577E0275}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
@@ -506,20 +608,20 @@
     <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
+    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
@@ -527,117 +629,185 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
         <v>23</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B19" r:id="rId1" display="https://www.digikey.ca/en/products/detail/gc-electronics/CT-4071-1R/6616089" xr:uid="{AECF80FD-C2D4-224B-A98C-24ACA50F6842}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Initial component placement process
</commit_message>
<xml_diff>
--- a/bom_panel.xlsx
+++ b/bom_panel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erudy/work/audio-power-amplifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B94326F-497A-B44D-8A00-EC53E175A9E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285895C3-AEC5-A343-A420-5E3A732A9104}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="460" windowWidth="27260" windowHeight="17200" xr2:uid="{8D4FBC5B-1539-A94D-B39E-707D1787DD7B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Description</t>
   </si>
@@ -171,6 +171,45 @@
   </si>
   <si>
     <t>1217861-1</t>
+  </si>
+  <si>
+    <t>Power Distribution wire</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>22759/32-12-0</t>
+  </si>
+  <si>
+    <t>22759/32-12-0-DS-ND</t>
+  </si>
+  <si>
+    <t>12 AWG Hook-Up Wire 37/28 Black 600V Enter Number of Feet in Order Quantity</t>
+  </si>
+  <si>
+    <t>81044/12-12-9</t>
+  </si>
+  <si>
+    <t>A132407-DS-ND</t>
+  </si>
+  <si>
+    <t>12 AWG Hook-Up, Dual Wall Wire 37/28 White 600V Enter Number of Feet in Order Quantity</t>
+  </si>
+  <si>
+    <t>12 AWG Hook-Up Wire 37/28 Brown 600V Enter Number of Feet in Order Quantity</t>
+  </si>
+  <si>
+    <t>55A0111-12-1-DS-ND</t>
+  </si>
+  <si>
+    <t>55A0111-12-1</t>
   </si>
 </sst>
 </file>
@@ -592,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E91B0B06-BA42-2340-A589-1662577E0275}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C19" sqref="C19:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -762,51 +801,98 @@
         <v>12</v>
       </c>
     </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B25" t="s">
         <v>16</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C25" t="s">
         <v>17</v>
       </c>
-      <c r="D20">
+      <c r="D25">
         <v>1</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E25" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B19" r:id="rId1" display="https://www.digikey.ca/en/products/detail/gc-electronics/CT-4071-1R/6616089" xr:uid="{AECF80FD-C2D4-224B-A98C-24ACA50F6842}"/>
+    <hyperlink ref="B24" r:id="rId1" display="https://www.digikey.ca/en/products/detail/gc-electronics/CT-4071-1R/6616089" xr:uid="{AECF80FD-C2D4-224B-A98C-24ACA50F6842}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added 3rd design iteration
</commit_message>
<xml_diff>
--- a/bom_panel.xlsx
+++ b/bom_panel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erudy/work/audio-power-amplifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1E40B3-502F-9741-8D67-510A820EF0FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259359AB-0E2F-5F43-A0E4-EF5F5988735C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="27260" windowHeight="17200" xr2:uid="{8D4FBC5B-1539-A94D-B39E-707D1787DD7B}"/>
+    <workbookView xWindow="32000" yWindow="1240" windowWidth="27260" windowHeight="17200" xr2:uid="{8D4FBC5B-1539-A94D-B39E-707D1787DD7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Description</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>55A0111-12-1</t>
+  </si>
+  <si>
+    <t>Primary side splice</t>
+  </si>
+  <si>
+    <t>36-8383-ND</t>
+  </si>
+  <si>
+    <t>Terminal Inline, Tap Connector IDC 14-16 to 18-20 AWG Blue</t>
   </si>
 </sst>
 </file>
@@ -309,13 +318,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -633,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E91B0B06-BA42-2340-A589-1662577E0275}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -848,6 +860,23 @@
         <v>56</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="6">
+        <v>8383</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Added mounting holes to amplifier PCB
</commit_message>
<xml_diff>
--- a/bom_panel.xlsx
+++ b/bom_panel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erudy/work/audio-power-amplifier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259359AB-0E2F-5F43-A0E4-EF5F5988735C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC39873-A406-004F-B097-7DBFEEBE55E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32000" yWindow="1240" windowWidth="27260" windowHeight="17200" xr2:uid="{8D4FBC5B-1539-A94D-B39E-707D1787DD7B}"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{8D4FBC5B-1539-A94D-B39E-707D1787DD7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>Description</t>
   </si>
@@ -128,15 +128,6 @@
     <t>Fuse</t>
   </si>
   <si>
-    <t>2-520181-2</t>
-  </si>
-  <si>
-    <t>0.187" (4.75mm) Quick Connect Female 18-22 AWG Crimp Connector Fully Insulated</t>
-  </si>
-  <si>
-    <t>A27804CT-ND</t>
-  </si>
-  <si>
     <t>A27831-ND</t>
   </si>
   <si>
@@ -219,6 +210,36 @@
   </si>
   <si>
     <t>Terminal Inline, Tap Connector IDC 14-16 to 18-20 AWG Blue</t>
+  </si>
+  <si>
+    <t>0.250" (6.35mm) Quick Connect Male  Solder Connector Non-Insulated</t>
+  </si>
+  <si>
+    <t>Primary side wire</t>
+  </si>
+  <si>
+    <t>55A0111-14-9</t>
+  </si>
+  <si>
+    <t>A132382-DS-ND</t>
+  </si>
+  <si>
+    <t>14 AWG Hook-Up Wire 19/27 White 600V Enter Number of Feet in Order Quantity</t>
+  </si>
+  <si>
+    <t>0.187" (4.75mm) Quick Connect Female 14-16 AWG Crimp Connector Fully Insulated</t>
+  </si>
+  <si>
+    <t>A99878CT-ND</t>
+  </si>
+  <si>
+    <t>3-520276-2</t>
+  </si>
+  <si>
+    <t>0.8 mm thick</t>
+  </si>
+  <si>
+    <t>0.8mm</t>
   </si>
 </sst>
 </file>
@@ -318,7 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -328,6 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -643,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E91B0B06-BA42-2340-A589-1662577E0275}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -681,7 +703,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -739,7 +761,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -751,7 +773,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -766,32 +788,38 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
+        <v>66</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>64</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -801,127 +829,148 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14">
         <v>12</v>
       </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>46</v>
+      <c r="A15" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" t="s">
-        <v>50</v>
-      </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B19" s="6">
         <v>8383</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
       <c r="E19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>22</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B29" t="s">
         <v>16</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C29" t="s">
         <v>17</v>
       </c>
-      <c r="D25">
+      <c r="D29">
         <v>1</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E29" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B24" r:id="rId1" display="https://www.digikey.ca/en/products/detail/gc-electronics/CT-4071-1R/6616089" xr:uid="{AECF80FD-C2D4-224B-A98C-24ACA50F6842}"/>
+    <hyperlink ref="B28" r:id="rId1" display="https://www.digikey.ca/en/products/detail/gc-electronics/CT-4071-1R/6616089" xr:uid="{AECF80FD-C2D4-224B-A98C-24ACA50F6842}"/>
+    <hyperlink ref="B11" r:id="rId2" display="https://www.digikey.ca/en/products/detail/te-connectivity-amp-connectors/3-520276-2/2060928" xr:uid="{949FCC7D-7E59-5848-82FA-AD47297F5E87}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>